<commit_message>
might delete second b7 code, replace with better first b7 code
</commit_message>
<xml_diff>
--- a/secondScan.xlsx
+++ b/secondScan.xlsx
@@ -369,7 +369,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -417,6 +417,90 @@
         </is>
       </c>
     </row>
+    <row r="2" spans="1:8" customFormat="false">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>74311420</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>80725555</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2019-05-20</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>invitation</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>bandapp</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>ios</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>74311420</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" spans="1:8" customFormat="false">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>74311420</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>80763028</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>US</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2019-05-22</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>invitation</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>bandapp</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>ios</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>74311420</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>